<commit_message>
Excel to mySQL Done!!!
</commit_message>
<xml_diff>
--- a/admin/Classes/test.xlsx
+++ b/admin/Classes/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08126349-8789-4916-8272-DB72293A5A8F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEAC16F-224E-4CED-9623-A332525B510D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
   <si>
     <t>ahmed</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>mohamad</t>
+  </si>
+  <si>
+    <t>joma</t>
+  </si>
+  <si>
+    <t>suli</t>
   </si>
 </sst>
 </file>
@@ -346,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:D11"/>
+  <dimension ref="A4:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,6 +472,20 @@
         <v>3453443</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>8948583</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>